<commit_message>
merging forecasting script with the UI update
</commit_message>
<xml_diff>
--- a/code/RESERVE_input_v1.xlsx
+++ b/code/RESERVE_input_v1.xlsx
@@ -5,32 +5,28 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuchi\PycharmProjects\new-modeling-toolkit\new_modeling_toolkit\reclaim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuchi\PycharmProjects\RESERVE\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE2C6EE-4DE4-49D8-BB54-E9FAEA5B908A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5EFA49-D5B8-4AF1-A95B-EB246456A950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="820" activeTab="5" xr2:uid="{9DEC9F6F-A494-4E03-A122-2B858774388B}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="820" activeTab="2" xr2:uid="{9DEC9F6F-A494-4E03-A122-2B858774388B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="33" r:id="rId1"/>
     <sheet name="Timeseries Attributes" sheetId="34" r:id="rId2"/>
-    <sheet name="Starts and Ends" sheetId="35" r:id="rId3"/>
-    <sheet name="Lag Term Configs" sheetId="36" r:id="rId4"/>
-    <sheet name="Lead Term Configs" sheetId="39" r:id="rId5"/>
-    <sheet name="Temporal Features" sheetId="37" r:id="rId6"/>
-    <sheet name="Main Parameters" sheetId="38" r:id="rId7"/>
+    <sheet name="Forecast Configs" sheetId="41" r:id="rId3"/>
+    <sheet name="Starts and Ends" sheetId="35" r:id="rId4"/>
+    <sheet name="Lag Term Configs" sheetId="36" r:id="rId5"/>
+    <sheet name="Lead Term Configs" sheetId="39" r:id="rId6"/>
+    <sheet name="Temporal Features" sheetId="37" r:id="rId7"/>
+    <sheet name="Main Parameters" sheetId="38" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="__FDS_HYPERLINK_TOGGLE_STATE__" hidden="1">"ON"</definedName>
     <definedName name="_Order1" hidden="1">255</definedName>
     <definedName name="_Order2" hidden="1">255</definedName>
-    <definedName name="IQ_CH">110000</definedName>
-    <definedName name="IQ_CQ">5000</definedName>
-    <definedName name="IQ_CY">10000</definedName>
-    <definedName name="IQ_DAILY">500000</definedName>
-    <definedName name="IQ_FH">100000</definedName>
-    <definedName name="IQ_FQ">500</definedName>
+    <definedName name="feature_names">OFFSET('Timeseries Attributes'!$A$2,,,num_features)</definedName>
     <definedName name="IQ_FWD_CY" hidden="1">10001</definedName>
     <definedName name="IQ_FWD_CY1" hidden="1">10002</definedName>
     <definedName name="IQ_FWD_CY2" hidden="1">10003</definedName>
@@ -40,17 +36,14 @@
     <definedName name="IQ_FWD_Q" hidden="1">501</definedName>
     <definedName name="IQ_FWD_Q1" hidden="1">502</definedName>
     <definedName name="IQ_FWD_Q2" hidden="1">503</definedName>
-    <definedName name="IQ_FY">1000</definedName>
     <definedName name="IQ_LATESTK" hidden="1">1000</definedName>
     <definedName name="IQ_LATESTQ" hidden="1">500</definedName>
-    <definedName name="IQ_LTM">2000</definedName>
     <definedName name="IQ_LTMMONTH" hidden="1">120000</definedName>
-    <definedName name="IQ_MONTH">15000</definedName>
-    <definedName name="IQ_NTM">6000</definedName>
     <definedName name="IQ_TODAY" hidden="1">0</definedName>
-    <definedName name="IQ_WEEK">50000</definedName>
-    <definedName name="IQ_YTD">3000</definedName>
     <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
+    <definedName name="is_feature_input">OFFSET('Timeseries Attributes'!$C$2,,,num_features)</definedName>
+    <definedName name="is_feature_output">OFFSET('Timeseries Attributes'!$D$2,,,num_features)</definedName>
+    <definedName name="num_features">COUNTA('Timeseries Attributes'!$A:$A)-1</definedName>
   </definedNames>
   <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
@@ -69,8 +62,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="78">
   <si>
     <t>Tab name</t>
   </si>
@@ -91,15 +106,6 @@
   </si>
   <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>Site_23019_wind_speed_wtk.csv</t>
-  </si>
-  <si>
-    <t>Wind_u_comp_Riverside_1.csv</t>
-  </si>
-  <si>
-    <t>Wind_v_comp_Riverside_1.csv</t>
   </si>
   <si>
     <t>Start Time</t>
@@ -190,63 +196,9 @@
     <t>The input files each contains one time series. For the specific application of RESERVE, it should include at least 6 files, the actuals and short-term forecasts of load, solar, and wind.</t>
   </si>
   <si>
-    <t>The wind speed from the wind tool kit of site 23019</t>
-  </si>
-  <si>
-    <t>The u component wind speed from the nearby ERA5 site</t>
-  </si>
-  <si>
-    <t>The v component wind speed from the nearby ERA5 site</t>
-  </si>
-  <si>
     <t>Sample Interval</t>
   </si>
   <si>
-    <t>wind_speed_WTK</t>
-  </si>
-  <si>
-    <t>U_wind_ERA5_loc_1</t>
-  </si>
-  <si>
-    <t>V_wind_ERA5_loc_1</t>
-  </si>
-  <si>
-    <t>U_wind_ERA5_loc_2</t>
-  </si>
-  <si>
-    <t>V_wind_ERA5_loc_2</t>
-  </si>
-  <si>
-    <t>U_wind_ERA5_loc_3</t>
-  </si>
-  <si>
-    <t>V_wind_ERA5_loc_3</t>
-  </si>
-  <si>
-    <t>U_wind_ERA5_loc_4</t>
-  </si>
-  <si>
-    <t>V_wind_ERA5_loc_4</t>
-  </si>
-  <si>
-    <t>Wind_u_comp_Riverside_2.csv</t>
-  </si>
-  <si>
-    <t>Wind_u_comp_Riverside_3.csv</t>
-  </si>
-  <si>
-    <t>Wind_v_comp_Riverside_3.csv</t>
-  </si>
-  <si>
-    <t>Wind_u_comp_Riverside_4.csv</t>
-  </si>
-  <si>
-    <t>Wind_v_comp_Riverside_4.csv</t>
-  </si>
-  <si>
-    <t>Wind_v_comp_Riverside_2.csv</t>
-  </si>
-  <si>
     <t>for example, if only caring about renewable forecast error, then holiday and weekday information should hold no value. If you want solar azimuth angle you must provide a valid longitude. If you want solar zenith angle then in addition to longitude you must have latitude as well</t>
   </si>
   <si>
@@ -284,6 +236,93 @@
   </si>
   <si>
     <t>Is Output?</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Forecast or Actual?</t>
+  </si>
+  <si>
+    <t>Generation or Load</t>
+  </si>
+  <si>
+    <t>Generation</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>synthesize forecast error</t>
+  </si>
+  <si>
+    <t>whether or not to synthesize forecast error from given time series.</t>
+  </si>
+  <si>
+    <t>Synthesize Forecast?</t>
+  </si>
+  <si>
+    <t>persistence</t>
+  </si>
+  <si>
+    <t>Lead Time</t>
+  </si>
+  <si>
+    <t>15M</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>wind</t>
+  </si>
+  <si>
+    <t>load_actuals</t>
+  </si>
+  <si>
+    <t>Load_RTD_Forecast.csv</t>
+  </si>
+  <si>
+    <t>Load</t>
+  </si>
+  <si>
+    <t>load_forecasts</t>
+  </si>
+  <si>
+    <t>Load_RTPD_Forecast.csv</t>
+  </si>
+  <si>
+    <t>Forecast</t>
+  </si>
+  <si>
+    <t>solar_actuals</t>
+  </si>
+  <si>
+    <t>Solar_RTD_Forecast.csv</t>
+  </si>
+  <si>
+    <t>wind_actuals</t>
+  </si>
+  <si>
+    <t>Wind_RTD_Forecast.csv</t>
+  </si>
+  <si>
+    <t>load</t>
+  </si>
+  <si>
+    <t>solar</t>
+  </si>
+  <si>
+    <t>actual load output downloaded from oasis</t>
+  </si>
+  <si>
+    <t>Load forecast in the RTPD downloaded from OASIS</t>
+  </si>
+  <si>
+    <t>solar actuals downloaded from OASIS</t>
+  </si>
+  <si>
+    <t>wind actuals downloaded from OASIS</t>
   </si>
 </sst>
 </file>
@@ -1353,14 +1392,14 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="131.875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.75" style="1"/>
+    <col min="2" max="2" width="131.8984375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.69921875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1371,12 +1410,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="22.8">
+    <row r="2" spans="1:2" ht="23">
       <c r="A2" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1387,28 +1426,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="91.2">
+    <row r="4" spans="1:2" ht="92">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="57">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="57.5">
       <c r="A5" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="22.8">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="23">
       <c r="A6" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1428,62 +1467,83 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="18.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.75" style="1"/>
+    <col min="1" max="1" width="18.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.19921875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.3984375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="47.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:8">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="C2" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="D2" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="E2" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="C3" s="6" t="b">
         <v>1</v>
@@ -1491,16 +1551,25 @@
       <c r="D3" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="E3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="5" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="C4" s="6" t="b">
         <v>1</v>
@@ -1508,16 +1577,25 @@
       <c r="D4" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="E4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="5" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="C5" s="6" t="b">
         <v>1</v>
@@ -1525,99 +1603,79 @@
       <c r="D5" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="E5" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="F5" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D8" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="G5" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D10" xr:uid="{EFAB30FF-DFD5-4C3B-BE7D-065C8C30091F}">
       <formula1>"True, False"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10" xr:uid="{8489B391-BA5B-43BB-B428-8325D605C9CB}">
+      <formula1>"Generation, Load"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F10" xr:uid="{C53729DF-3843-447A-88E0-15C860A037B7}">
+      <formula1>"Forecast, Actual"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1626,6 +1684,154 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A4587E-D5AA-44CF-BBF4-C44CD0B5D2EC}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.5"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="27.8984375" customWidth="1"/>
+    <col min="5" max="5" width="46.796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="13">
+      <c r="A1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="A2:A5" ca="1">feature_names</f>
+        <v>load_actuals</v>
+      </c>
+      <c r="B2" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="4" t="str">
+        <f ca="1"/>
+        <v>load_forecasts</v>
+      </c>
+      <c r="B3" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="4" t="str">
+        <f ca="1"/>
+        <v>solar_actuals</v>
+      </c>
+      <c r="B4" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4" t="str">
+        <f ca="1"/>
+        <v>wind_actuals</v>
+      </c>
+      <c r="B5" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="4"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="4"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="4"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="4"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B10" xr:uid="{89C35547-612E-4B59-B90F-39484FC49142}">
+      <formula1>"True, False"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C10" xr:uid="{9A404CA3-3BBD-49D1-8F23-D3D0E8CA7E7A}">
+      <formula1>"persistence, solar persistence"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E09AC71-0441-43EC-994B-FB3EC6D446EC}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -1633,27 +1839,27 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="25.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.75" style="1" customWidth="1"/>
-    <col min="4" max="4" width="65.625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.75" style="1"/>
+    <col min="1" max="1" width="25.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.69921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.69921875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="65.59765625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.69921875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>6</v>
@@ -1661,44 +1867,44 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" s="7">
-        <v>39083</v>
+        <v>42736</v>
       </c>
       <c r="C2" s="7">
-        <v>40544</v>
+        <v>43466</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3" s="7">
-        <v>40909</v>
+        <v>43466</v>
       </c>
       <c r="C3" s="7">
-        <v>41275</v>
+        <v>43831</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B4" s="7">
-        <v>39083</v>
+        <v>42736</v>
       </c>
       <c r="C4" s="7">
-        <v>41275</v>
+        <v>43831</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1707,7 +1913,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF60C23A-811A-4465-86A0-B683DF075A41}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -1715,32 +1921,33 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="18.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.75" style="1"/>
+    <col min="1" max="1" width="18.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.69921875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="5" t="s">
-        <v>43</v>
+      <c r="A2" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="A2:A5" ca="1">IF(is_feature_input, feature_names,"")</f>
+        <v>load_actuals</v>
       </c>
       <c r="B2" s="5">
         <v>-2</v>
@@ -1753,8 +1960,9 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="5" t="s">
-        <v>44</v>
+      <c r="A3" s="4" t="str">
+        <f ca="1"/>
+        <v>load_forecasts</v>
       </c>
       <c r="B3" s="5">
         <v>-2</v>
@@ -1767,8 +1975,9 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="5" t="s">
-        <v>45</v>
+      <c r="A4" s="4" t="str">
+        <f ca="1"/>
+        <v>solar_actuals</v>
       </c>
       <c r="B4" s="5">
         <v>-2</v>
@@ -1781,8 +1990,9 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="5" t="s">
-        <v>46</v>
+      <c r="A5" s="4" t="str">
+        <f ca="1"/>
+        <v>wind_actuals</v>
       </c>
       <c r="B5" s="5">
         <v>-2</v>
@@ -1795,110 +2005,28 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="5">
-        <v>-2</v>
-      </c>
-      <c r="C6" s="5">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5">
-        <v>1</v>
-      </c>
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="5">
-        <v>-2</v>
-      </c>
-      <c r="C7" s="5">
-        <v>1</v>
-      </c>
-      <c r="D7" s="5">
-        <v>1</v>
-      </c>
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="5">
-        <v>-2</v>
-      </c>
-      <c r="C8" s="5">
-        <v>1</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1</v>
-      </c>
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="5">
-        <v>-2</v>
-      </c>
-      <c r="C9" s="5">
-        <v>1</v>
-      </c>
-      <c r="D9" s="5">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E09AC4AA-C461-4500-B671-42317969ABF1}">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4"/>
-  <cols>
-    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="13.2">
-      <c r="A1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="12">
-      <c r="A2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="5">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5">
-        <v>2</v>
-      </c>
-      <c r="D2" s="5">
-        <v>2</v>
-      </c>
-      <c r="E2" s="9"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1906,30 +2034,93 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E09AC4AA-C461-4500-B671-42317969ABF1}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.5"/>
+  <cols>
+    <col min="1" max="1" width="15.69921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="13">
+      <c r="A1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="13">
+      <c r="A2" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="A2:A5" ca="1">IF(is_feature_output,feature_names,"")</f>
+        <v/>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12890C65-6643-49AC-AF35-926FCA64FE19}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="28.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.8984375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="65" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.75" style="1"/>
+    <col min="4" max="16384" width="8.69921875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>6</v>
@@ -1937,7 +2128,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="4" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="B2" s="5" t="b">
         <v>1</v>
@@ -1946,7 +2137,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="B3" s="5" t="b">
         <v>1</v>
@@ -1955,7 +2146,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="4" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="B4" s="5" t="b">
         <v>1</v>
@@ -1964,7 +2155,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="B5" s="5" t="b">
         <v>1</v>
@@ -1973,7 +2164,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="4" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="B6" s="5" t="b">
         <v>1</v>
@@ -1982,7 +2173,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="4" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="B7" s="5" t="b">
         <v>1</v>
@@ -2001,31 +2192,31 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD5CEF0-F20A-458E-B05B-C17F22A3B0F2}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="22.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="67" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.75" style="1"/>
+    <col min="4" max="16384" width="8.69921875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>6</v>
@@ -2033,53 +2224,64 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="5">
-        <v>37</v>
+        <v>30</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B3" s="5">
-        <v>-116.35</v>
+        <v>37</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B4" s="5">
-        <v>-8</v>
-      </c>
-      <c r="C4" s="5"/>
+        <v>-116.35</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
+      </c>
+      <c r="B5" s="5">
+        <v>-8</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
+      </c>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2098,17 +2300,29 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000A8EBF2820B64B4EB9D32959209F47BE" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1df5dac8d2b4244012f33bd0d3237b4f">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dfc47abc-3033-4421-9d18-1d4465274a5d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0ed33b1377eba927b234e6e5873f2048" ns2:_="">
-    <xsd:import namespace="dfc47abc-3033-4421-9d18-1d4465274a5d"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010072B5728302353E4D9CE5235E951EDC1A" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="80a8e38918c9aefec6303039bf3ae9f9">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="af4d241c-2181-49e7-b6a6-88a8d7ebb8c2" xmlns:ns4="037e2d66-b6e1-454a-beb1-c40c580ba142" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e2415cd808c9b5f72f957eb2a95870d1" ns3:_="" ns4:_="">
+    <xsd:import namespace="af4d241c-2181-49e7-b6a6-88a8d7ebb8c2"/>
+    <xsd:import namespace="037e2d66-b6e1-454a-beb1-c40c580ba142"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element name="documentManagement">
             <xsd:complexType>
               <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns3:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -2116,17 +2330,96 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="dfc47abc-3033-4421-9d18-1d4465274a5d" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="af4d241c-2181-49e7-b6a6-88a8d7ebb8c2" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="10" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="037e2d66-b6e1-454a-beb1-c40c580ba142" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+    <xsd:element name="MediaServiceFastMetadata" ma:index="12" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="13" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="14" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="15" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="19" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="20" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -2244,13 +2537,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A775AB7-AAF4-4D0D-91D0-858D293F5100}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21C876F0-81E3-484C-BB22-323BE62444C6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="dfc47abc-3033-4421-9d18-1d4465274a5d"/>
+    <ds:schemaRef ds:uri="af4d241c-2181-49e7-b6a6-88a8d7ebb8c2"/>
+    <ds:schemaRef ds:uri="037e2d66-b6e1-454a-beb1-c40c580ba142"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -2264,15 +2558,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{331B2F40-BE42-4A7E-82C9-31BDAE1A21B2}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="037e2d66-b6e1-454a-beb1-c40c580ba142"/>
+    <ds:schemaRef ds:uri="af4d241c-2181-49e7-b6a6-88a8d7ebb8c2"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="dfc47abc-3033-4421-9d18-1d4465274a5d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Reconciliation of capital and lowercase letters
1. In data_preprocessing.py: capitalize initials of "_forecast_error" or "net_load_forecast_error" to be consistent with visualization parameters in rescue.ipynb.
2. In UI: capitalize Category column (column H) in "Timeseries Attributes" tab to be consistent with visualization parameters in rescue.ipynb
</commit_message>
<xml_diff>
--- a/code/RESERVE_input_v1.xlsx
+++ b/code/RESERVE_input_v1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuchi\PycharmProjects\RESERVE\code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruoshui.li\Documents\GitHub\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF251595-4AE2-4612-9C60-81D68C786399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6987E265-558B-437F-933E-E534E1496483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="744" yWindow="1116" windowWidth="18096" windowHeight="9696" tabRatio="820" activeTab="2" xr2:uid="{9DEC9F6F-A494-4E03-A122-2B858774388B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="820" activeTab="1" xr2:uid="{9DEC9F6F-A494-4E03-A122-2B858774388B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="33" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="83">
   <si>
     <t>Tab name</t>
   </si>
@@ -262,9 +262,6 @@
     <t>Category</t>
   </si>
   <si>
-    <t>wind</t>
-  </si>
-  <si>
     <t>load_actuals</t>
   </si>
   <si>
@@ -295,12 +292,6 @@
     <t>Wind_RTD_Forecast.csv</t>
   </si>
   <si>
-    <t>load</t>
-  </si>
-  <si>
-    <t>solar</t>
-  </si>
-  <si>
     <t>actual load output downloaded from oasis</t>
   </si>
   <si>
@@ -341,6 +332,12 @@
   </si>
   <si>
     <t>solar persistence</t>
+  </si>
+  <si>
+    <t>Solar</t>
+  </si>
+  <si>
+    <t>Wind</t>
   </si>
 </sst>
 </file>
@@ -1487,8 +1484,8 @@
   </sheetPr>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="14"/>
@@ -1519,13 +1516,13 @@
         <v>46</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>48</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>56</v>
@@ -1536,10 +1533,10 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="C2" s="6" t="b">
         <v>1</v>
@@ -1551,24 +1548,24 @@
         <v>1</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>50</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="C3" s="6" t="b">
         <v>1</v>
@@ -1580,24 +1577,24 @@
         <v>1</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>65</v>
       </c>
       <c r="C4" s="6" t="b">
         <v>1</v>
@@ -1615,18 +1612,18 @@
         <v>50</v>
       </c>
       <c r="H4" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>67</v>
       </c>
       <c r="C5" s="6" t="b">
         <v>1</v>
@@ -1644,10 +1641,10 @@
         <v>50</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1729,7 +1726,7 @@
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1758,13 +1755,13 @@
         <v>55</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>6</v>
@@ -1782,7 +1779,7 @@
         <v>54</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E2" s="5">
         <v>-2</v>
@@ -1807,7 +1804,7 @@
         <v>54</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E3" s="5">
         <v>-2</v>
@@ -1829,10 +1826,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E4" s="5">
         <v>-2</v>
@@ -1857,7 +1854,7 @@
         <v>54</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E5" s="5">
         <v>-2</v>
@@ -2329,7 +2326,7 @@
         <v>28</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>22</v>
@@ -2371,7 +2368,7 @@
         <v>33</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C6" s="5"/>
     </row>
@@ -2388,13 +2385,13 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2627,18 +2624,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2661,14 +2658,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0721155-47D6-477F-9A2B-C20E8BCCE367}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{331B2F40-BE42-4A7E-82C9-31BDAE1A21B2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2683,4 +2672,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0721155-47D6-477F-9A2B-C20E8BCCE367}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
bug fixes. Move functions outside of data_preprocessing.py
</commit_message>
<xml_diff>
--- a/code/RESERVE_input_v1.xlsx
+++ b/code/RESERVE_input_v1.xlsx
@@ -8,24 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuchi\PycharmProjects\RESERVE\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF251595-4AE2-4612-9C60-81D68C786399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F7F960-DC6B-43CD-9F4A-D26CF06D78C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="744" yWindow="1116" windowWidth="18096" windowHeight="9696" tabRatio="820" activeTab="2" xr2:uid="{9DEC9F6F-A494-4E03-A122-2B858774388B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="820" activeTab="1" xr2:uid="{9DEC9F6F-A494-4E03-A122-2B858774388B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="33" r:id="rId1"/>
-    <sheet name="Timeseries Attributes" sheetId="34" r:id="rId2"/>
-    <sheet name="Forecast Configs" sheetId="41" r:id="rId3"/>
+    <sheet name="Main Parameters" sheetId="38" r:id="rId2"/>
+    <sheet name="Timeseries Attributes" sheetId="34" r:id="rId3"/>
     <sheet name="Starts and Ends" sheetId="35" r:id="rId4"/>
     <sheet name="Lag Term Configs" sheetId="36" r:id="rId5"/>
     <sheet name="Lead Term Configs" sheetId="39" r:id="rId6"/>
     <sheet name="Temporal Features" sheetId="37" r:id="rId7"/>
-    <sheet name="Main Parameters" sheetId="38" r:id="rId8"/>
+    <sheet name="Forecast Configs" sheetId="41" r:id="rId8"/>
+    <sheet name="Forecast Error Configs" sheetId="43" r:id="rId9"/>
+    <sheet name="Forecast Error Contribution" sheetId="42" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="__FDS_HYPERLINK_TOGGLE_STATE__" hidden="1">"ON"</definedName>
     <definedName name="_Order1" hidden="1">255</definedName>
     <definedName name="_Order2" hidden="1">255</definedName>
+    <definedName name="fe_categories">OFFSET('Forecast Error Contribution'!$E$2,,,num_features)</definedName>
     <definedName name="feature_names">OFFSET('Timeseries Attributes'!$A$2,,,num_features)</definedName>
     <definedName name="IQ_FWD_CY" hidden="1">10001</definedName>
     <definedName name="IQ_FWD_CY1" hidden="1">10002</definedName>
@@ -85,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="89">
   <si>
     <t>Tab name</t>
   </si>
@@ -238,67 +241,103 @@
     <t>Generation or Load</t>
   </si>
   <si>
+    <t>synthesize forecast error</t>
+  </si>
+  <si>
+    <t>whether or not to synthesize forecast error from given time series.</t>
+  </si>
+  <si>
+    <t>Synthesize Forecast?</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Impacts Forecast Error?</t>
+  </si>
+  <si>
+    <t>Forecast Horizon</t>
+  </si>
+  <si>
+    <t>Forecast Feature Name</t>
+  </si>
+  <si>
+    <t>Forecast Term Step</t>
+  </si>
+  <si>
+    <t>Forecast Term Start</t>
+  </si>
+  <si>
+    <t>Forecast Term End</t>
+  </si>
+  <si>
+    <t>Category Name</t>
+  </si>
+  <si>
+    <t>Error Lead Term Start</t>
+  </si>
+  <si>
+    <t>Error Lead Term End</t>
+  </si>
+  <si>
+    <t>Error Lead Term Step</t>
+  </si>
+  <si>
+    <t>Synthesize Error?</t>
+  </si>
+  <si>
+    <t>load_actuals</t>
+  </si>
+  <si>
+    <t>Load_RTD_Forecast.csv</t>
+  </si>
+  <si>
+    <t>load_forecasts</t>
+  </si>
+  <si>
+    <t>Load_RTPD_Forecast.csv</t>
+  </si>
+  <si>
+    <t>solar_actuals</t>
+  </si>
+  <si>
+    <t>Solar_RTD_Forecast.csv</t>
+  </si>
+  <si>
+    <t>wind_actuals</t>
+  </si>
+  <si>
+    <t>Wind_RTD_Forecast.csv</t>
+  </si>
+  <si>
+    <t>15T</t>
+  </si>
+  <si>
+    <t>persistence</t>
+  </si>
+  <si>
+    <t>solar persistence</t>
+  </si>
+  <si>
+    <t>45T</t>
+  </si>
+  <si>
+    <t>Load</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Forecast</t>
+  </si>
+  <si>
     <t>Generation</t>
   </si>
   <si>
-    <t>Actual</t>
-  </si>
-  <si>
-    <t>synthesize forecast error</t>
-  </si>
-  <si>
-    <t>whether or not to synthesize forecast error from given time series.</t>
-  </si>
-  <si>
-    <t>Synthesize Forecast?</t>
-  </si>
-  <si>
-    <t>persistence</t>
-  </si>
-  <si>
-    <t>Lead Time</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>wind</t>
-  </si>
-  <si>
-    <t>load_actuals</t>
-  </si>
-  <si>
-    <t>Load_RTD_Forecast.csv</t>
-  </si>
-  <si>
-    <t>Load</t>
-  </si>
-  <si>
-    <t>load_forecasts</t>
-  </si>
-  <si>
-    <t>Load_RTPD_Forecast.csv</t>
-  </si>
-  <si>
-    <t>Forecast</t>
-  </si>
-  <si>
-    <t>solar_actuals</t>
-  </si>
-  <si>
-    <t>Solar_RTD_Forecast.csv</t>
-  </si>
-  <si>
-    <t>wind_actuals</t>
-  </si>
-  <si>
-    <t>Wind_RTD_Forecast.csv</t>
-  </si>
-  <si>
-    <t>load</t>
-  </si>
-  <si>
-    <t>solar</t>
+    <t>Solar</t>
+  </si>
+  <si>
+    <t>Wind</t>
   </si>
   <si>
     <t>actual load output downloaded from oasis</t>
@@ -313,34 +352,13 @@
     <t>wind actuals downloaded from OASIS</t>
   </si>
   <si>
-    <t>Lag Start</t>
-  </si>
-  <si>
-    <t>Lag End</t>
-  </si>
-  <si>
-    <t>Lag Step</t>
-  </si>
-  <si>
-    <t>The amount of look ahead (in sample interval), for this prediction problem</t>
-  </si>
-  <si>
-    <t>synthesized forecast error lead</t>
-  </si>
-  <si>
-    <t>Impacts Forecast Error?</t>
-  </si>
-  <si>
-    <t>15T</t>
-  </si>
-  <si>
-    <t>RESERVE_PSE_0.1</t>
+    <t>RESERVE_PSE_1.0</t>
   </si>
   <si>
     <t>Forecast or Actual</t>
   </si>
   <si>
-    <t>solar persistence</t>
+    <t>Net Load Forecast Error</t>
   </si>
 </sst>
 </file>
@@ -1002,7 +1020,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1032,6 +1050,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="21">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="1" xfId="53">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1405,19 +1429,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE957269-E51E-4FF7-BEFD-D977BC54FDC1}">
   <sheetPr>
-    <tabColor rgb="FFC00000"/>
+    <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="131.8984375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.69921875" style="1"/>
+    <col min="2" max="2" width="131.875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.75" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1428,7 +1452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="23">
+    <row r="2" spans="1:2" ht="22.8">
       <c r="A2" s="4" t="s">
         <v>18</v>
       </c>
@@ -1444,7 +1468,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="92">
+    <row r="4" spans="1:2" ht="91.2">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1452,7 +1476,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="57.5">
+    <row r="5" spans="1:2" ht="57">
       <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
@@ -1460,7 +1484,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="23">
+    <row r="6" spans="1:2" ht="22.8">
       <c r="A6" s="4" t="s">
         <v>25</v>
       </c>
@@ -1480,32 +1504,307 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90E83A58-69E0-406E-AFDF-FC6F2092B946}">
+  <sheetPr>
+    <tabColor theme="2"/>
+  </sheetPr>
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.4"/>
+  <cols>
+    <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="13.2">
+      <c r="A1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="A2:A5" ca="1">feature_names</f>
+        <v>load_actuals</v>
+      </c>
+      <c r="B2" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="4" t="str">
+        <f ca="1"/>
+        <v>load_forecasts</v>
+      </c>
+      <c r="B3" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="4" t="str">
+        <f ca="1"/>
+        <v>solar_actuals</v>
+      </c>
+      <c r="B4" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="4" t="str">
+        <f ca="1"/>
+        <v>wind_actuals</v>
+      </c>
+      <c r="B5" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="4"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="4"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="4"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="4"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="4"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D10" xr:uid="{BB66B291-ADBA-401D-ACA5-5AD063576B6E}">
+      <formula1>"Forecast, Actual, N.A."</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C10" xr:uid="{BCAF3030-C03C-45FE-B219-8778F704C8EE}">
+      <formula1>"Generation, Load, N.A."</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B10" xr:uid="{E1984AC6-DD34-47AD-9A78-B0EE5CA8ECCE}">
+      <formula1>"True, False"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD5CEF0-F20A-458E-B05B-C17F22A3B0F2}">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="22.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="67" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.75" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="5">
+        <v>37</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="5">
+        <v>-116.35</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="5">
+        <v>-8</v>
+      </c>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="2" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{792C6F83-7CA1-407A-BC09-36AF288B5A32}">
   <sheetPr>
-    <tabColor rgb="FFFFC000"/>
+    <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="18.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.19921875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.3984375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="47.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.69921875" style="1"/>
+    <col min="1" max="1" width="18.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.25" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -1519,27 +1818,15 @@
         <v>46</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C2" s="6" t="b">
         <v>1</v>
@@ -1547,28 +1834,16 @@
       <c r="D2" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="E2" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="E2" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C3" s="6" t="b">
         <v>1</v>
@@ -1576,28 +1851,16 @@
       <c r="D3" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="E3" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="E3" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="B4" s="5" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C4" s="6" t="b">
         <v>1</v>
@@ -1605,28 +1868,16 @@
       <c r="D4" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="E4" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="E4" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C5" s="6" t="b">
         <v>1</v>
@@ -1634,87 +1885,49 @@
       <c r="D5" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="E5" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="E5" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+      <c r="E10" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:E10" xr:uid="{EFAB30FF-DFD5-4C3B-BE7D-065C8C30091F}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D10" xr:uid="{15EE09A2-6117-48D5-B137-9CB2F823C2AA}">
       <formula1>"True, False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F10" xr:uid="{8489B391-BA5B-43BB-B428-8325D605C9CB}">
-      <formula1>"Generation, Load, N.A."</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G10" xr:uid="{C53729DF-3843-447A-88E0-15C860A037B7}">
-      <formula1>"Forecast, Actual, N.A."</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1722,34 +1935,379 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E09AC71-0441-43EC-994B-FB3EC6D446EC}">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="25.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.75" style="1" customWidth="1"/>
+    <col min="4" max="4" width="65.625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.75" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="7">
+        <v>42736</v>
+      </c>
+      <c r="C2" s="7">
+        <v>43466</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="7">
+        <v>43466</v>
+      </c>
+      <c r="C3" s="7">
+        <v>43831</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="7">
+        <v>42736</v>
+      </c>
+      <c r="C4" s="7">
+        <v>43831</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="2" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF60C23A-811A-4465-86A0-B683DF075A41}">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="18.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="8.75" style="1"/>
+    <col min="7" max="7" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.75" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="A2:A5" ca="1">_xlfn._xlws.FILTER(feature_names, is_feature_input)</f>
+        <v>load_actuals</v>
+      </c>
+      <c r="B2" s="5">
+        <v>-5</v>
+      </c>
+      <c r="C2" s="5">
+        <v>-2</v>
+      </c>
+      <c r="D2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="4" t="str">
+        <f ca="1"/>
+        <v>load_forecasts</v>
+      </c>
+      <c r="B3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="4" t="str">
+        <f ca="1"/>
+        <v>solar_actuals</v>
+      </c>
+      <c r="B4" s="5">
+        <v>-5</v>
+      </c>
+      <c r="C4" s="5">
+        <v>-2</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="4" t="str">
+        <f ca="1"/>
+        <v>wind_actuals</v>
+      </c>
+      <c r="B5" s="5">
+        <v>-5</v>
+      </c>
+      <c r="C5" s="5">
+        <v>-2</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E09AC4AA-C461-4500-B671-42317969ABF1}">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.4"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="13.2">
+      <c r="A1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="12">
+      <c r="A2" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="A2" ca="1">IFERROR(_xlfn._xlws.FILTER(feature_names,is_feature_output),"")</f>
+        <v/>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12890C65-6643-49AC-AF35-926FCA64FE19}">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="28.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.75" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="10"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="2" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A4587E-D5AA-44CF-BBF4-C44CD0B5D2EC}">
   <sheetPr>
-    <tabColor rgb="FFFFC000"/>
+    <tabColor theme="2"/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.8984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="27.8984375" customWidth="1"/>
-    <col min="5" max="5" width="10.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="46.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="27.875" customWidth="1"/>
+    <col min="6" max="6" width="20.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="46.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13">
+    <row r="1" spans="1:9" ht="13.2">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>47</v>
@@ -1758,19 +2316,22 @@
         <v>55</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="11.5">
+    <row r="2" spans="1:9" ht="11.4">
       <c r="A2" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="A2:A5" ca="1">feature_names</f>
         <v>load_actuals</v>
@@ -1778,24 +2339,18 @@
       <c r="B2" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E2" s="5">
-        <v>-2</v>
-      </c>
-      <c r="F2" s="5">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5">
-        <v>1</v>
-      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="11" t="str">
+        <f>IF(B2, _xlfn.CONCAT($A2,"_forecast"),"")</f>
+        <v/>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
       <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" ht="11.5">
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" ht="11.4">
       <c r="A3" s="4" t="str">
         <f ca="1"/>
         <v>load_forecasts</v>
@@ -1803,24 +2358,18 @@
       <c r="B3" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" s="5">
-        <v>-2</v>
-      </c>
-      <c r="F3" s="5">
-        <v>1</v>
-      </c>
-      <c r="G3" s="5">
-        <v>1</v>
-      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="11" t="str">
+        <f t="shared" ref="D3:D10" si="0">IF(B3, _xlfn.CONCAT($A3,"_forecast"),"")</f>
+        <v/>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
       <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:8" ht="11.5">
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" ht="11.4">
       <c r="A4" s="4" t="str">
         <f ca="1"/>
         <v>solar_actuals</v>
@@ -1829,23 +2378,27 @@
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" s="5">
-        <v>-2</v>
+        <v>74</v>
+      </c>
+      <c r="D4" s="11" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>solar_actuals_forecast</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>75</v>
       </c>
       <c r="F4" s="5">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G4" s="5">
         <v>1</v>
       </c>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" ht="11.5">
+      <c r="H4" s="5">
+        <v>1</v>
+      </c>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" ht="11.4">
       <c r="A5" s="4" t="str">
         <f ca="1"/>
         <v>wind_actuals</v>
@@ -1854,71 +2407,95 @@
         <v>1</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E5" s="5">
-        <v>-2</v>
+        <v>73</v>
+      </c>
+      <c r="D5" s="11" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>wind_actuals_forecast</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>75</v>
       </c>
       <c r="F5" s="5">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G5" s="5">
         <v>1</v>
       </c>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" ht="11.5">
+      <c r="H5" s="5">
+        <v>1</v>
+      </c>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" ht="11.4">
       <c r="A6" s="4"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="5"/>
+      <c r="D6" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" ht="11.5">
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" ht="11.4">
       <c r="A7" s="4"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="5"/>
+      <c r="D7" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" ht="11.5">
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" ht="11.4">
       <c r="A8" s="4"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="5"/>
+      <c r="D8" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" ht="11.5">
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" ht="11.4">
       <c r="A9" s="4"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="5"/>
+      <c r="D9" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" ht="11.5">
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" ht="11.4">
       <c r="A10" s="4"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
-      <c r="D10" s="5"/>
+      <c r="D10" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -1933,141 +2510,67 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E09AC71-0441-43EC-994B-FB3EC6D446EC}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A5C0621-C379-46AE-A583-8F458E1A2E8C}">
   <sheetPr>
-    <tabColor rgb="FFFFC000"/>
+    <tabColor theme="2"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="11.4"/>
   <cols>
-    <col min="1" max="1" width="25.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.69921875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.69921875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="65.59765625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.69921875" style="1"/>
+    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5" ht="13.2">
       <c r="A1" s="3" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="7">
-        <v>42736</v>
-      </c>
-      <c r="C2" s="7">
-        <v>43466</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="7">
-        <v>43466</v>
-      </c>
-      <c r="C3" s="7">
-        <v>43831</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="7">
-        <v>42736</v>
-      </c>
-      <c r="C4" s="7">
-        <v>43831</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="2" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF60C23A-811A-4465-86A0-B683DF075A41}">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1:D9"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="14"/>
-  <cols>
-    <col min="1" max="1" width="18.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.69921875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="4" t="str" cm="1">
-        <f t="array" aca="1" ref="A2:A5" ca="1">IF(is_feature_input, feature_names,"")</f>
-        <v>load_actuals</v>
-      </c>
-      <c r="B2" s="5">
-        <v>-2</v>
+        <v>61</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="C2" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="4" t="str">
-        <f ca="1"/>
-        <v>load_forecasts</v>
-      </c>
-      <c r="B3" s="5">
-        <v>-2</v>
+      <c r="E2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="A3:A5" ca="1">_xlfn.UNIQUE(fe_categories)</f>
+        <v>Load</v>
+      </c>
+      <c r="B3" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="C3" s="5">
         <v>1</v>
@@ -2075,331 +2578,98 @@
       <c r="D3" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="4" t="str">
         <f ca="1"/>
-        <v>solar_actuals</v>
-      </c>
-      <c r="B4" s="5">
-        <v>-2</v>
+        <v>Solar</v>
+      </c>
+      <c r="B4" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="C4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="4" t="str">
         <f ca="1"/>
-        <v>wind_actuals</v>
-      </c>
-      <c r="B5" s="5">
-        <v>-2</v>
+        <v>Wind</v>
+      </c>
+      <c r="B5" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="C5" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="4"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C11" xr:uid="{0F06FF99-8C65-43F1-AF74-CE63CC761799}">
+      <formula1>"persistence, solar persistence, N.A."</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B11" xr:uid="{3E3FF154-6465-45A1-9F3C-18949730F937}">
+      <formula1>"True, False"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E09AC4AA-C461-4500-B671-42317969ABF1}">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.5"/>
-  <cols>
-    <col min="1" max="1" width="15.69921875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="13">
-      <c r="A1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="13">
-      <c r="A2" s="4" t="str" cm="1">
-        <f t="array" aca="1" ref="A2:A5" ca="1">IF(is_feature_output,feature_names,"")</f>
-        <v/>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="9"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12890C65-6643-49AC-AF35-926FCA64FE19}">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1:C9"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="14"/>
-  <cols>
-    <col min="1" max="1" width="28.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.69921875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="10"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="10"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="2" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD5CEF0-F20A-458E-B05B-C17F22A3B0F2}">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="14"/>
-  <cols>
-    <col min="1" max="1" width="22.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.59765625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="67" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.69921875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="5">
-        <v>37</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="5">
-        <v>-116.35</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="5">
-        <v>-8</v>
-      </c>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" s="5">
-        <v>1</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="2" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Bug fix for visualization
</commit_message>
<xml_diff>
--- a/code/RESERVE_input_v1.xlsx
+++ b/code/RESERVE_input_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuchi\PycharmProjects\RESERVE\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F7F960-DC6B-43CD-9F4A-D26CF06D78C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081B5A7C-1451-456A-AD46-ACD6EC78978E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="820" activeTab="1" xr2:uid="{9DEC9F6F-A494-4E03-A122-2B858774388B}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="34580" windowHeight="13980" tabRatio="820" activeTab="1" xr2:uid="{9DEC9F6F-A494-4E03-A122-2B858774388B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="33" r:id="rId1"/>
@@ -1693,7 +1693,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8"/>
@@ -2674,6 +2674,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010072B5728302353E4D9CE5235E951EDC1A" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="80a8e38918c9aefec6303039bf3ae9f9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="af4d241c-2181-49e7-b6a6-88a8d7ebb8c2" xmlns:ns4="037e2d66-b6e1-454a-beb1-c40c580ba142" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e2415cd808c9b5f72f957eb2a95870d1" ns3:_="" ns4:_="">
     <xsd:import namespace="af4d241c-2181-49e7-b6a6-88a8d7ebb8c2"/>
@@ -2896,22 +2911,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{331B2F40-BE42-4A7E-82C9-31BDAE1A21B2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="037e2d66-b6e1-454a-beb1-c40c580ba142"/>
+    <ds:schemaRef ds:uri="af4d241c-2181-49e7-b6a6-88a8d7ebb8c2"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0721155-47D6-477F-9A2B-C20E8BCCE367}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21C876F0-81E3-484C-BB22-323BE62444C6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2928,29 +2953,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0721155-47D6-477F-9A2B-C20E8BCCE367}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{331B2F40-BE42-4A7E-82C9-31BDAE1A21B2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="037e2d66-b6e1-454a-beb1-c40c580ba142"/>
-    <ds:schemaRef ds:uri="af4d241c-2181-49e7-b6a6-88a8d7ebb8c2"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update 1axis tracking solar persistence
</commit_message>
<xml_diff>
--- a/code/RESERVE_input_v1.xlsx
+++ b/code/RESERVE_input_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuchi\PycharmProjects\RESERVE\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081B5A7C-1451-456A-AD46-ACD6EC78978E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87071368-444B-4810-AEBF-3318683F816C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="34580" windowHeight="13980" tabRatio="820" activeTab="1" xr2:uid="{9DEC9F6F-A494-4E03-A122-2B858774388B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="820" activeTab="1" xr2:uid="{9DEC9F6F-A494-4E03-A122-2B858774388B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="33" r:id="rId1"/>
@@ -289,27 +289,15 @@
     <t>load_actuals</t>
   </si>
   <si>
-    <t>Load_RTD_Forecast.csv</t>
-  </si>
-  <si>
     <t>load_forecasts</t>
   </si>
   <si>
-    <t>Load_RTPD_Forecast.csv</t>
-  </si>
-  <si>
     <t>solar_actuals</t>
   </si>
   <si>
-    <t>Solar_RTD_Forecast.csv</t>
-  </si>
-  <si>
     <t>wind_actuals</t>
   </si>
   <si>
-    <t>Wind_RTD_Forecast.csv</t>
-  </si>
-  <si>
     <t>15T</t>
   </si>
   <si>
@@ -352,13 +340,25 @@
     <t>wind actuals downloaded from OASIS</t>
   </si>
   <si>
-    <t>RESERVE_PSE_1.0</t>
-  </si>
-  <si>
     <t>Forecast or Actual</t>
   </si>
   <si>
     <t>Net Load Forecast Error</t>
+  </si>
+  <si>
+    <t>PSE_RTD_load_forecast_scaled.csv</t>
+  </si>
+  <si>
+    <t>PSE_RTPD_load_forecast_scaled.csv</t>
+  </si>
+  <si>
+    <t>PSE_solar_5_minute_actuals.csv</t>
+  </si>
+  <si>
+    <t>PSE_wind_5_minute_actuals.csv</t>
+  </si>
+  <si>
+    <t>RESERVE_PSE_6.0</t>
   </si>
 </sst>
 </file>
@@ -1512,7 +1512,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.4"/>
@@ -1536,7 +1536,7 @@
         <v>48</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>52</v>
@@ -1554,16 +1554,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1575,16 +1575,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1596,16 +1596,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1617,16 +1617,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1693,7 +1693,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8"/>
@@ -1720,7 +1720,7 @@
         <v>28</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>22</v>
@@ -1731,7 +1731,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="5">
-        <v>37</v>
+        <v>45.9</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>36</v>
@@ -1742,7 +1742,7 @@
         <v>26</v>
       </c>
       <c r="B4" s="5">
-        <v>-116.35</v>
+        <v>-106.62</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>36</v>
@@ -1762,7 +1762,7 @@
         <v>33</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C6" s="5"/>
     </row>
@@ -1791,7 +1791,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8"/>
@@ -1826,7 +1826,7 @@
         <v>64</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="C2" s="6" t="b">
         <v>1</v>
@@ -1835,15 +1835,15 @@
         <v>0</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="C3" s="6" t="b">
         <v>1</v>
@@ -1852,15 +1852,15 @@
         <v>0</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="C4" s="6" t="b">
         <v>1</v>
@@ -1869,15 +1869,15 @@
         <v>0</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="C5" s="6" t="b">
         <v>1</v>
@@ -1886,7 +1886,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1943,7 +1943,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8"/>
@@ -2287,8 +2287,8 @@
   </sheetPr>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2378,14 +2378,14 @@
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D4" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>solar_actuals_forecast</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F4" s="5">
         <v>-1</v>
@@ -2407,14 +2407,14 @@
         <v>1</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D5" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>wind_actuals_forecast</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F5" s="5">
         <v>-1</v>
@@ -2518,7 +2518,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.4"/>
@@ -2549,7 +2549,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="12" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B2" s="6" t="b">
         <v>1</v>
@@ -2674,18 +2674,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2912,6 +2912,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0721155-47D6-477F-9A2B-C20E8BCCE367}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{331B2F40-BE42-4A7E-82C9-31BDAE1A21B2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2924,14 +2932,6 @@
     <ds:schemaRef ds:uri="037e2d66-b6e1-454a-beb1-c40c580ba142"/>
     <ds:schemaRef ds:uri="af4d241c-2181-49e7-b6a6-88a8d7ebb8c2"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0721155-47D6-477F-9A2B-C20E8BCCE367}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>